<commit_message>
moved to selenium 2.53.1
</commit_message>
<xml_diff>
--- a/src/test/resources/SampleDataFile.xlsx
+++ b/src/test/resources/SampleDataFile.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="VERIFY_TABLE_DATA" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>USERNAME</t>
   </si>
@@ -24,10 +24,16 @@
     <t>PASSWORD</t>
   </si>
   <si>
-    <t>UserName1</t>
-  </si>
-  <si>
-    <t>Password1</t>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>P2</t>
   </si>
 </sst>
 </file>
@@ -75,6 +81,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -122,7 +131,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -157,7 +166,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -366,19 +375,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B3"/>
+  <dimension ref="A2:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -386,12 +395,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -405,7 +422,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -417,7 +434,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>